<commit_message>
Update to user-data to fix Uganda missing entities
</commit_message>
<xml_diff>
--- a/user-data/uganda-avg-house-size/uganda-avg-house-size.xlsx
+++ b/user-data/uganda-avg-house-size/uganda-avg-house-size.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="242">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -31,337 +31,673 @@
     <t xml:space="preserve">d101</t>
   </si>
   <si>
+    <t xml:space="preserve">Kalangala</t>
+  </si>
+  <si>
     <t xml:space="preserve">d102</t>
   </si>
   <si>
+    <t xml:space="preserve">Kampala</t>
+  </si>
+  <si>
     <t xml:space="preserve">d103</t>
   </si>
   <si>
+    <t xml:space="preserve">Kiboga</t>
+  </si>
+  <si>
     <t xml:space="preserve">d104</t>
   </si>
   <si>
+    <t xml:space="preserve">Luwero</t>
+  </si>
+  <si>
     <t xml:space="preserve">d105</t>
   </si>
   <si>
+    <t xml:space="preserve">Masaka</t>
+  </si>
+  <si>
     <t xml:space="preserve">d106</t>
   </si>
   <si>
+    <t xml:space="preserve">Mpigi</t>
+  </si>
+  <si>
     <t xml:space="preserve">d107</t>
   </si>
   <si>
+    <t xml:space="preserve">Mubende</t>
+  </si>
+  <si>
     <t xml:space="preserve">d108</t>
   </si>
   <si>
+    <t xml:space="preserve">Mukono</t>
+  </si>
+  <si>
     <t xml:space="preserve">d109</t>
   </si>
   <si>
+    <t xml:space="preserve">Nakasongola</t>
+  </si>
+  <si>
     <t xml:space="preserve">d110</t>
   </si>
   <si>
+    <t xml:space="preserve">Rakai</t>
+  </si>
+  <si>
     <t xml:space="preserve">d111</t>
   </si>
   <si>
+    <t xml:space="preserve">Ssembabule</t>
+  </si>
+  <si>
     <t xml:space="preserve">d112</t>
   </si>
   <si>
+    <t xml:space="preserve">Kayunga</t>
+  </si>
+  <si>
     <t xml:space="preserve">d113</t>
   </si>
   <si>
+    <t xml:space="preserve">Wakiso</t>
+  </si>
+  <si>
     <t xml:space="preserve">d114</t>
   </si>
   <si>
+    <t xml:space="preserve">Lyantonde</t>
+  </si>
+  <si>
     <t xml:space="preserve">d115</t>
   </si>
   <si>
+    <t xml:space="preserve">Mityana</t>
+  </si>
+  <si>
     <t xml:space="preserve">d116</t>
   </si>
   <si>
+    <t xml:space="preserve">Nakaseke</t>
+  </si>
+  <si>
     <t xml:space="preserve">d117</t>
   </si>
   <si>
+    <t xml:space="preserve">Buikwe</t>
+  </si>
+  <si>
     <t xml:space="preserve">d118</t>
   </si>
   <si>
+    <t xml:space="preserve">Bukomansimbi</t>
+  </si>
+  <si>
     <t xml:space="preserve">d119</t>
   </si>
   <si>
+    <t xml:space="preserve">Butambala</t>
+  </si>
+  <si>
     <t xml:space="preserve">d120</t>
   </si>
   <si>
+    <t xml:space="preserve">Buvuma</t>
+  </si>
+  <si>
     <t xml:space="preserve">d121</t>
   </si>
   <si>
+    <t xml:space="preserve">Gomba</t>
+  </si>
+  <si>
     <t xml:space="preserve">d122</t>
   </si>
   <si>
+    <t xml:space="preserve">Kalungu</t>
+  </si>
+  <si>
     <t xml:space="preserve">d123</t>
   </si>
   <si>
+    <t xml:space="preserve">Kyankwanzi</t>
+  </si>
+  <si>
     <t xml:space="preserve">d124</t>
   </si>
   <si>
+    <t xml:space="preserve">Lwengo</t>
+  </si>
+  <si>
     <t xml:space="preserve">d201</t>
   </si>
   <si>
+    <t xml:space="preserve">Bugiri</t>
+  </si>
+  <si>
     <t xml:space="preserve">d202</t>
   </si>
   <si>
+    <t xml:space="preserve">Busia</t>
+  </si>
+  <si>
     <t xml:space="preserve">d203</t>
   </si>
   <si>
+    <t xml:space="preserve">Iganga</t>
+  </si>
+  <si>
     <t xml:space="preserve">d204</t>
   </si>
   <si>
+    <t xml:space="preserve">Jinja</t>
+  </si>
+  <si>
     <t xml:space="preserve">d205</t>
   </si>
   <si>
+    <t xml:space="preserve">Kamuli</t>
+  </si>
+  <si>
     <t xml:space="preserve">d206</t>
   </si>
   <si>
+    <t xml:space="preserve">Kapchorwa</t>
+  </si>
+  <si>
     <t xml:space="preserve">d207</t>
   </si>
   <si>
+    <t xml:space="preserve">Katakwi</t>
+  </si>
+  <si>
     <t xml:space="preserve">d208</t>
   </si>
   <si>
+    <t xml:space="preserve">Kumi</t>
+  </si>
+  <si>
     <t xml:space="preserve">d209</t>
   </si>
   <si>
+    <t xml:space="preserve">Mbale</t>
+  </si>
+  <si>
     <t xml:space="preserve">d210</t>
   </si>
   <si>
+    <t xml:space="preserve">Pallisa</t>
+  </si>
+  <si>
     <t xml:space="preserve">d211</t>
   </si>
   <si>
+    <t xml:space="preserve">Soroti</t>
+  </si>
+  <si>
     <t xml:space="preserve">d212</t>
   </si>
   <si>
+    <t xml:space="preserve">Tororo</t>
+  </si>
+  <si>
     <t xml:space="preserve">d213</t>
   </si>
   <si>
+    <t xml:space="preserve">Kaberamaido</t>
+  </si>
+  <si>
     <t xml:space="preserve">d214</t>
   </si>
   <si>
+    <t xml:space="preserve">Mayuge</t>
+  </si>
+  <si>
     <t xml:space="preserve">d215</t>
   </si>
   <si>
+    <t xml:space="preserve">Sironko</t>
+  </si>
+  <si>
     <t xml:space="preserve">d216</t>
   </si>
   <si>
+    <t xml:space="preserve">Amuria</t>
+  </si>
+  <si>
     <t xml:space="preserve">d217</t>
   </si>
   <si>
+    <t xml:space="preserve">Budaka</t>
+  </si>
+  <si>
     <t xml:space="preserve">d218</t>
   </si>
   <si>
+    <t xml:space="preserve">Bududa</t>
+  </si>
+  <si>
     <t xml:space="preserve">d219</t>
   </si>
   <si>
+    <t xml:space="preserve">Bukedea</t>
+  </si>
+  <si>
     <t xml:space="preserve">d220</t>
   </si>
   <si>
+    <t xml:space="preserve">Bukwo</t>
+  </si>
+  <si>
     <t xml:space="preserve">d221</t>
   </si>
   <si>
+    <t xml:space="preserve">Butaleja</t>
+  </si>
+  <si>
     <t xml:space="preserve">d222</t>
   </si>
   <si>
+    <t xml:space="preserve">Kaliro</t>
+  </si>
+  <si>
     <t xml:space="preserve">d223</t>
   </si>
   <si>
+    <t xml:space="preserve">Manafwa</t>
+  </si>
+  <si>
     <t xml:space="preserve">d224</t>
   </si>
   <si>
+    <t xml:space="preserve">Namutumba</t>
+  </si>
+  <si>
     <t xml:space="preserve">d225</t>
   </si>
   <si>
+    <t xml:space="preserve">Bulambuli</t>
+  </si>
+  <si>
     <t xml:space="preserve">d226</t>
   </si>
   <si>
+    <t xml:space="preserve">Buyende</t>
+  </si>
+  <si>
     <t xml:space="preserve">d227</t>
   </si>
   <si>
+    <t xml:space="preserve">Kibuku</t>
+  </si>
+  <si>
     <t xml:space="preserve">d228</t>
   </si>
   <si>
+    <t xml:space="preserve">Kween</t>
+  </si>
+  <si>
     <t xml:space="preserve">d229</t>
   </si>
   <si>
+    <t xml:space="preserve">Luuka</t>
+  </si>
+  <si>
     <t xml:space="preserve">d230</t>
   </si>
   <si>
+    <t xml:space="preserve">Namayingo</t>
+  </si>
+  <si>
     <t xml:space="preserve">d231</t>
   </si>
   <si>
+    <t xml:space="preserve">Ngora</t>
+  </si>
+  <si>
     <t xml:space="preserve">d232</t>
   </si>
   <si>
+    <t xml:space="preserve">Serere</t>
+  </si>
+  <si>
     <t xml:space="preserve">d301</t>
   </si>
   <si>
+    <t xml:space="preserve">Adjumani</t>
+  </si>
+  <si>
     <t xml:space="preserve">d302</t>
   </si>
   <si>
+    <t xml:space="preserve">Apac</t>
+  </si>
+  <si>
     <t xml:space="preserve">d303</t>
   </si>
   <si>
+    <t xml:space="preserve">Arua</t>
+  </si>
+  <si>
     <t xml:space="preserve">d304</t>
   </si>
   <si>
+    <t xml:space="preserve">Gulu</t>
+  </si>
+  <si>
     <t xml:space="preserve">d305</t>
   </si>
   <si>
+    <t xml:space="preserve">Kitgum</t>
+  </si>
+  <si>
     <t xml:space="preserve">d306</t>
   </si>
   <si>
+    <t xml:space="preserve">Kotido</t>
+  </si>
+  <si>
     <t xml:space="preserve">d307</t>
   </si>
   <si>
+    <t xml:space="preserve">Lira</t>
+  </si>
+  <si>
     <t xml:space="preserve">d308</t>
   </si>
   <si>
+    <t xml:space="preserve">Moroto</t>
+  </si>
+  <si>
     <t xml:space="preserve">d309</t>
   </si>
   <si>
+    <t xml:space="preserve">Moyo</t>
+  </si>
+  <si>
     <t xml:space="preserve">d310</t>
   </si>
   <si>
+    <t xml:space="preserve">Nebbi</t>
+  </si>
+  <si>
     <t xml:space="preserve">d311</t>
   </si>
   <si>
+    <t xml:space="preserve">Nakapiripirit</t>
+  </si>
+  <si>
     <t xml:space="preserve">d312</t>
   </si>
   <si>
+    <t xml:space="preserve">Pader</t>
+  </si>
+  <si>
     <t xml:space="preserve">d313</t>
   </si>
   <si>
+    <t xml:space="preserve">Yumbe</t>
+  </si>
+  <si>
     <t xml:space="preserve">d314</t>
   </si>
   <si>
+    <t xml:space="preserve">Abim</t>
+  </si>
+  <si>
     <t xml:space="preserve">d315</t>
   </si>
   <si>
+    <t xml:space="preserve">Amolatar</t>
+  </si>
+  <si>
     <t xml:space="preserve">d316</t>
   </si>
   <si>
+    <t xml:space="preserve">Amuru</t>
+  </si>
+  <si>
     <t xml:space="preserve">d317</t>
   </si>
   <si>
+    <t xml:space="preserve">Dokolo</t>
+  </si>
+  <si>
     <t xml:space="preserve">d318</t>
   </si>
   <si>
+    <t xml:space="preserve">Kaabong</t>
+  </si>
+  <si>
     <t xml:space="preserve">d319</t>
   </si>
   <si>
+    <t xml:space="preserve">Koboko</t>
+  </si>
+  <si>
     <t xml:space="preserve">d320</t>
   </si>
   <si>
+    <t xml:space="preserve">Maracha</t>
+  </si>
+  <si>
     <t xml:space="preserve">d321</t>
   </si>
   <si>
+    <t xml:space="preserve">Oyam</t>
+  </si>
+  <si>
     <t xml:space="preserve">d322</t>
   </si>
   <si>
+    <t xml:space="preserve">Agago</t>
+  </si>
+  <si>
     <t xml:space="preserve">d323</t>
   </si>
   <si>
+    <t xml:space="preserve">Alebtong</t>
+  </si>
+  <si>
     <t xml:space="preserve">d324</t>
   </si>
   <si>
+    <t xml:space="preserve">Amudat</t>
+  </si>
+  <si>
     <t xml:space="preserve">d325</t>
   </si>
   <si>
+    <t xml:space="preserve">Kole</t>
+  </si>
+  <si>
     <t xml:space="preserve">d326</t>
   </si>
   <si>
+    <t xml:space="preserve">Lamwo</t>
+  </si>
+  <si>
     <t xml:space="preserve">d327</t>
   </si>
   <si>
+    <t xml:space="preserve">Napak</t>
+  </si>
+  <si>
     <t xml:space="preserve">d328</t>
   </si>
   <si>
+    <t xml:space="preserve">Nwoya</t>
+  </si>
+  <si>
     <t xml:space="preserve">d329</t>
   </si>
   <si>
+    <t xml:space="preserve">Otuke</t>
+  </si>
+  <si>
     <t xml:space="preserve">d330</t>
   </si>
   <si>
+    <t xml:space="preserve">Zombo</t>
+  </si>
+  <si>
     <t xml:space="preserve">d401</t>
   </si>
   <si>
+    <t xml:space="preserve">Bundibugyo</t>
+  </si>
+  <si>
     <t xml:space="preserve">d402</t>
   </si>
   <si>
+    <t xml:space="preserve">Bushenyi</t>
+  </si>
+  <si>
     <t xml:space="preserve">d403</t>
   </si>
   <si>
+    <t xml:space="preserve">Hoima</t>
+  </si>
+  <si>
     <t xml:space="preserve">d404</t>
   </si>
   <si>
+    <t xml:space="preserve">Kabale</t>
+  </si>
+  <si>
     <t xml:space="preserve">d405</t>
   </si>
   <si>
+    <t xml:space="preserve">Kabarole</t>
+  </si>
+  <si>
     <t xml:space="preserve">d406</t>
   </si>
   <si>
+    <t xml:space="preserve">Kasese</t>
+  </si>
+  <si>
     <t xml:space="preserve">d407</t>
   </si>
   <si>
+    <t xml:space="preserve">Kibaale</t>
+  </si>
+  <si>
     <t xml:space="preserve">d408</t>
   </si>
   <si>
+    <t xml:space="preserve">Kisoro</t>
+  </si>
+  <si>
     <t xml:space="preserve">d409</t>
   </si>
   <si>
+    <t xml:space="preserve">Masindi</t>
+  </si>
+  <si>
     <t xml:space="preserve">d410</t>
   </si>
   <si>
+    <t xml:space="preserve">Mbarara</t>
+  </si>
+  <si>
     <t xml:space="preserve">d411</t>
   </si>
   <si>
+    <t xml:space="preserve">Ntungamo</t>
+  </si>
+  <si>
     <t xml:space="preserve">d412</t>
   </si>
   <si>
+    <t xml:space="preserve">Rukungiri</t>
+  </si>
+  <si>
     <t xml:space="preserve">d413</t>
   </si>
   <si>
+    <t xml:space="preserve">Kamwenge</t>
+  </si>
+  <si>
     <t xml:space="preserve">d414</t>
   </si>
   <si>
+    <t xml:space="preserve">Kanungu</t>
+  </si>
+  <si>
     <t xml:space="preserve">d415</t>
   </si>
   <si>
+    <t xml:space="preserve">Kyenjojo</t>
+  </si>
+  <si>
     <t xml:space="preserve">d416</t>
   </si>
   <si>
+    <t xml:space="preserve">Buliisa</t>
+  </si>
+  <si>
     <t xml:space="preserve">d417</t>
   </si>
   <si>
+    <t xml:space="preserve">Ibanda</t>
+  </si>
+  <si>
     <t xml:space="preserve">d418</t>
   </si>
   <si>
+    <t xml:space="preserve">Isingiro</t>
+  </si>
+  <si>
     <t xml:space="preserve">d419</t>
   </si>
   <si>
+    <t xml:space="preserve">Kiruhura</t>
+  </si>
+  <si>
     <t xml:space="preserve">d420</t>
   </si>
   <si>
+    <t xml:space="preserve">Buhweju</t>
+  </si>
+  <si>
     <t xml:space="preserve">d421</t>
   </si>
   <si>
+    <t xml:space="preserve">Kiryandongo</t>
+  </si>
+  <si>
     <t xml:space="preserve">d422</t>
   </si>
   <si>
+    <t xml:space="preserve">Kyegegwa</t>
+  </si>
+  <si>
     <t xml:space="preserve">d423</t>
   </si>
   <si>
+    <t xml:space="preserve">Mitooma</t>
+  </si>
+  <si>
     <t xml:space="preserve">d424</t>
   </si>
   <si>
+    <t xml:space="preserve">Ntoroko</t>
+  </si>
+  <si>
     <t xml:space="preserve">d425</t>
   </si>
   <si>
+    <t xml:space="preserve">Rubirizi</t>
+  </si>
+  <si>
     <t xml:space="preserve">d426</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sheema</t>
   </si>
   <si>
     <t xml:space="preserve">2014</t>
@@ -737,22 +1073,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>117</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5">
@@ -760,7 +1096,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7">
@@ -768,52 +1104,52 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>122</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>123</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>123</v>
+        <v>235</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>123</v>
+        <v>235</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>124</v>
+        <v>236</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>237</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>126</v>
+        <v>238</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>127</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>128</v>
+        <v>240</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>129</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -848,7 +1184,9 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2"/>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
       <c r="C2" t="n">
         <v>2014</v>
       </c>
@@ -858,9 +1196,11 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3"/>
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
       <c r="C3" t="n">
         <v>2014</v>
       </c>
@@ -870,9 +1210,11 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4"/>
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
       <c r="C4" t="n">
         <v>2014</v>
       </c>
@@ -882,9 +1224,11 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5"/>
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
       <c r="C5" t="n">
         <v>2014</v>
       </c>
@@ -894,9 +1238,11 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6"/>
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
       <c r="C6" t="n">
         <v>2014</v>
       </c>
@@ -906,9 +1252,11 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7"/>
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
       <c r="C7" t="n">
         <v>2014</v>
       </c>
@@ -918,9 +1266,11 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8"/>
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
       <c r="C8" t="n">
         <v>2014</v>
       </c>
@@ -930,9 +1280,11 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9"/>
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
       <c r="C9" t="n">
         <v>2014</v>
       </c>
@@ -942,9 +1294,11 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10"/>
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
       <c r="C10" t="n">
         <v>2014</v>
       </c>
@@ -954,9 +1308,11 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11"/>
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
       <c r="C11" t="n">
         <v>2014</v>
       </c>
@@ -966,9 +1322,11 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12"/>
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
       <c r="C12" t="n">
         <v>2014</v>
       </c>
@@ -978,9 +1336,11 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13"/>
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
       <c r="C13" t="n">
         <v>2014</v>
       </c>
@@ -990,9 +1350,11 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14"/>
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
       <c r="C14" t="n">
         <v>2014</v>
       </c>
@@ -1002,9 +1364,11 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15"/>
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
       <c r="C15" t="n">
         <v>2014</v>
       </c>
@@ -1014,9 +1378,11 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16"/>
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
       <c r="C16" t="n">
         <v>2014</v>
       </c>
@@ -1026,9 +1392,11 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17"/>
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
       <c r="C17" t="n">
         <v>2014</v>
       </c>
@@ -1038,9 +1406,11 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18"/>
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
       <c r="C18" t="n">
         <v>2014</v>
       </c>
@@ -1050,9 +1420,11 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19"/>
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
       <c r="C19" t="n">
         <v>2014</v>
       </c>
@@ -1062,9 +1434,11 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20"/>
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
       <c r="C20" t="n">
         <v>2014</v>
       </c>
@@ -1074,9 +1448,11 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21"/>
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
       <c r="C21" t="n">
         <v>2014</v>
       </c>
@@ -1086,9 +1462,11 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22"/>
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
+        <v>45</v>
+      </c>
       <c r="C22" t="n">
         <v>2014</v>
       </c>
@@ -1098,9 +1476,11 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23"/>
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
+        <v>47</v>
+      </c>
       <c r="C23" t="n">
         <v>2014</v>
       </c>
@@ -1110,9 +1490,11 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24"/>
+        <v>48</v>
+      </c>
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
       <c r="C24" t="n">
         <v>2014</v>
       </c>
@@ -1122,9 +1504,11 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25"/>
+        <v>50</v>
+      </c>
+      <c r="B25" t="s">
+        <v>51</v>
+      </c>
       <c r="C25" t="n">
         <v>2014</v>
       </c>
@@ -1134,9 +1518,11 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26"/>
+        <v>52</v>
+      </c>
+      <c r="B26" t="s">
+        <v>53</v>
+      </c>
       <c r="C26" t="n">
         <v>2014</v>
       </c>
@@ -1146,9 +1532,11 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27"/>
+        <v>54</v>
+      </c>
+      <c r="B27" t="s">
+        <v>55</v>
+      </c>
       <c r="C27" t="n">
         <v>2014</v>
       </c>
@@ -1158,9 +1546,11 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28"/>
+        <v>56</v>
+      </c>
+      <c r="B28" t="s">
+        <v>57</v>
+      </c>
       <c r="C28" t="n">
         <v>2014</v>
       </c>
@@ -1170,9 +1560,11 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29"/>
+        <v>58</v>
+      </c>
+      <c r="B29" t="s">
+        <v>59</v>
+      </c>
       <c r="C29" t="n">
         <v>2014</v>
       </c>
@@ -1182,9 +1574,11 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30"/>
+        <v>60</v>
+      </c>
+      <c r="B30" t="s">
+        <v>61</v>
+      </c>
       <c r="C30" t="n">
         <v>2014</v>
       </c>
@@ -1194,9 +1588,11 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>33</v>
-      </c>
-      <c r="B31"/>
+        <v>62</v>
+      </c>
+      <c r="B31" t="s">
+        <v>63</v>
+      </c>
       <c r="C31" t="n">
         <v>2014</v>
       </c>
@@ -1206,9 +1602,11 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32"/>
+        <v>64</v>
+      </c>
+      <c r="B32" t="s">
+        <v>65</v>
+      </c>
       <c r="C32" t="n">
         <v>2014</v>
       </c>
@@ -1218,9 +1616,11 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33"/>
+        <v>66</v>
+      </c>
+      <c r="B33" t="s">
+        <v>67</v>
+      </c>
       <c r="C33" t="n">
         <v>2014</v>
       </c>
@@ -1230,9 +1630,11 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34"/>
+        <v>68</v>
+      </c>
+      <c r="B34" t="s">
+        <v>69</v>
+      </c>
       <c r="C34" t="n">
         <v>2014</v>
       </c>
@@ -1242,9 +1644,11 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35"/>
+        <v>70</v>
+      </c>
+      <c r="B35" t="s">
+        <v>71</v>
+      </c>
       <c r="C35" t="n">
         <v>2014</v>
       </c>
@@ -1254,9 +1658,11 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36"/>
+        <v>72</v>
+      </c>
+      <c r="B36" t="s">
+        <v>73</v>
+      </c>
       <c r="C36" t="n">
         <v>2014</v>
       </c>
@@ -1266,9 +1672,11 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>39</v>
-      </c>
-      <c r="B37"/>
+        <v>74</v>
+      </c>
+      <c r="B37" t="s">
+        <v>75</v>
+      </c>
       <c r="C37" t="n">
         <v>2014</v>
       </c>
@@ -1278,9 +1686,11 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>40</v>
-      </c>
-      <c r="B38"/>
+        <v>76</v>
+      </c>
+      <c r="B38" t="s">
+        <v>77</v>
+      </c>
       <c r="C38" t="n">
         <v>2014</v>
       </c>
@@ -1290,9 +1700,11 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>41</v>
-      </c>
-      <c r="B39"/>
+        <v>78</v>
+      </c>
+      <c r="B39" t="s">
+        <v>79</v>
+      </c>
       <c r="C39" t="n">
         <v>2014</v>
       </c>
@@ -1302,9 +1714,11 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>42</v>
-      </c>
-      <c r="B40"/>
+        <v>80</v>
+      </c>
+      <c r="B40" t="s">
+        <v>81</v>
+      </c>
       <c r="C40" t="n">
         <v>2014</v>
       </c>
@@ -1314,9 +1728,11 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>43</v>
-      </c>
-      <c r="B41"/>
+        <v>82</v>
+      </c>
+      <c r="B41" t="s">
+        <v>83</v>
+      </c>
       <c r="C41" t="n">
         <v>2014</v>
       </c>
@@ -1326,9 +1742,11 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>44</v>
-      </c>
-      <c r="B42"/>
+        <v>84</v>
+      </c>
+      <c r="B42" t="s">
+        <v>85</v>
+      </c>
       <c r="C42" t="n">
         <v>2014</v>
       </c>
@@ -1338,9 +1756,11 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>45</v>
-      </c>
-      <c r="B43"/>
+        <v>86</v>
+      </c>
+      <c r="B43" t="s">
+        <v>87</v>
+      </c>
       <c r="C43" t="n">
         <v>2014</v>
       </c>
@@ -1350,9 +1770,11 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>46</v>
-      </c>
-      <c r="B44"/>
+        <v>88</v>
+      </c>
+      <c r="B44" t="s">
+        <v>89</v>
+      </c>
       <c r="C44" t="n">
         <v>2014</v>
       </c>
@@ -1362,9 +1784,11 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>47</v>
-      </c>
-      <c r="B45"/>
+        <v>90</v>
+      </c>
+      <c r="B45" t="s">
+        <v>91</v>
+      </c>
       <c r="C45" t="n">
         <v>2014</v>
       </c>
@@ -1374,9 +1798,11 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>48</v>
-      </c>
-      <c r="B46"/>
+        <v>92</v>
+      </c>
+      <c r="B46" t="s">
+        <v>93</v>
+      </c>
       <c r="C46" t="n">
         <v>2014</v>
       </c>
@@ -1386,9 +1812,11 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>49</v>
-      </c>
-      <c r="B47"/>
+        <v>94</v>
+      </c>
+      <c r="B47" t="s">
+        <v>95</v>
+      </c>
       <c r="C47" t="n">
         <v>2014</v>
       </c>
@@ -1398,9 +1826,11 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>50</v>
-      </c>
-      <c r="B48"/>
+        <v>96</v>
+      </c>
+      <c r="B48" t="s">
+        <v>97</v>
+      </c>
       <c r="C48" t="n">
         <v>2014</v>
       </c>
@@ -1410,9 +1840,11 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>51</v>
-      </c>
-      <c r="B49"/>
+        <v>98</v>
+      </c>
+      <c r="B49" t="s">
+        <v>99</v>
+      </c>
       <c r="C49" t="n">
         <v>2014</v>
       </c>
@@ -1422,9 +1854,11 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>52</v>
-      </c>
-      <c r="B50"/>
+        <v>100</v>
+      </c>
+      <c r="B50" t="s">
+        <v>101</v>
+      </c>
       <c r="C50" t="n">
         <v>2014</v>
       </c>
@@ -1434,9 +1868,11 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>53</v>
-      </c>
-      <c r="B51"/>
+        <v>102</v>
+      </c>
+      <c r="B51" t="s">
+        <v>103</v>
+      </c>
       <c r="C51" t="n">
         <v>2014</v>
       </c>
@@ -1446,9 +1882,11 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>54</v>
-      </c>
-      <c r="B52"/>
+        <v>104</v>
+      </c>
+      <c r="B52" t="s">
+        <v>105</v>
+      </c>
       <c r="C52" t="n">
         <v>2014</v>
       </c>
@@ -1458,9 +1896,11 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>55</v>
-      </c>
-      <c r="B53"/>
+        <v>106</v>
+      </c>
+      <c r="B53" t="s">
+        <v>107</v>
+      </c>
       <c r="C53" t="n">
         <v>2014</v>
       </c>
@@ -1470,9 +1910,11 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>56</v>
-      </c>
-      <c r="B54"/>
+        <v>108</v>
+      </c>
+      <c r="B54" t="s">
+        <v>109</v>
+      </c>
       <c r="C54" t="n">
         <v>2014</v>
       </c>
@@ -1482,9 +1924,11 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>57</v>
-      </c>
-      <c r="B55"/>
+        <v>110</v>
+      </c>
+      <c r="B55" t="s">
+        <v>111</v>
+      </c>
       <c r="C55" t="n">
         <v>2014</v>
       </c>
@@ -1494,9 +1938,11 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>58</v>
-      </c>
-      <c r="B56"/>
+        <v>112</v>
+      </c>
+      <c r="B56" t="s">
+        <v>113</v>
+      </c>
       <c r="C56" t="n">
         <v>2014</v>
       </c>
@@ -1506,9 +1952,11 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>59</v>
-      </c>
-      <c r="B57"/>
+        <v>114</v>
+      </c>
+      <c r="B57" t="s">
+        <v>115</v>
+      </c>
       <c r="C57" t="n">
         <v>2014</v>
       </c>
@@ -1518,9 +1966,11 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>60</v>
-      </c>
-      <c r="B58"/>
+        <v>116</v>
+      </c>
+      <c r="B58" t="s">
+        <v>117</v>
+      </c>
       <c r="C58" t="n">
         <v>2014</v>
       </c>
@@ -1530,9 +1980,11 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>61</v>
-      </c>
-      <c r="B59"/>
+        <v>118</v>
+      </c>
+      <c r="B59" t="s">
+        <v>119</v>
+      </c>
       <c r="C59" t="n">
         <v>2014</v>
       </c>
@@ -1542,9 +1994,11 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>62</v>
-      </c>
-      <c r="B60"/>
+        <v>120</v>
+      </c>
+      <c r="B60" t="s">
+        <v>121</v>
+      </c>
       <c r="C60" t="n">
         <v>2014</v>
       </c>
@@ -1554,9 +2008,11 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>63</v>
-      </c>
-      <c r="B61"/>
+        <v>122</v>
+      </c>
+      <c r="B61" t="s">
+        <v>123</v>
+      </c>
       <c r="C61" t="n">
         <v>2014</v>
       </c>
@@ -1566,9 +2022,11 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>64</v>
-      </c>
-      <c r="B62"/>
+        <v>124</v>
+      </c>
+      <c r="B62" t="s">
+        <v>125</v>
+      </c>
       <c r="C62" t="n">
         <v>2014</v>
       </c>
@@ -1578,9 +2036,11 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>65</v>
-      </c>
-      <c r="B63"/>
+        <v>126</v>
+      </c>
+      <c r="B63" t="s">
+        <v>127</v>
+      </c>
       <c r="C63" t="n">
         <v>2014</v>
       </c>
@@ -1590,9 +2050,11 @@
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>66</v>
-      </c>
-      <c r="B64"/>
+        <v>128</v>
+      </c>
+      <c r="B64" t="s">
+        <v>129</v>
+      </c>
       <c r="C64" t="n">
         <v>2014</v>
       </c>
@@ -1602,9 +2064,11 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>67</v>
-      </c>
-      <c r="B65"/>
+        <v>130</v>
+      </c>
+      <c r="B65" t="s">
+        <v>131</v>
+      </c>
       <c r="C65" t="n">
         <v>2014</v>
       </c>
@@ -1614,9 +2078,11 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>68</v>
-      </c>
-      <c r="B66"/>
+        <v>132</v>
+      </c>
+      <c r="B66" t="s">
+        <v>133</v>
+      </c>
       <c r="C66" t="n">
         <v>2014</v>
       </c>
@@ -1626,9 +2092,11 @@
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>69</v>
-      </c>
-      <c r="B67"/>
+        <v>134</v>
+      </c>
+      <c r="B67" t="s">
+        <v>135</v>
+      </c>
       <c r="C67" t="n">
         <v>2014</v>
       </c>
@@ -1638,9 +2106,11 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>70</v>
-      </c>
-      <c r="B68"/>
+        <v>136</v>
+      </c>
+      <c r="B68" t="s">
+        <v>137</v>
+      </c>
       <c r="C68" t="n">
         <v>2014</v>
       </c>
@@ -1650,9 +2120,11 @@
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>71</v>
-      </c>
-      <c r="B69"/>
+        <v>138</v>
+      </c>
+      <c r="B69" t="s">
+        <v>139</v>
+      </c>
       <c r="C69" t="n">
         <v>2014</v>
       </c>
@@ -1662,9 +2134,11 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>72</v>
-      </c>
-      <c r="B70"/>
+        <v>140</v>
+      </c>
+      <c r="B70" t="s">
+        <v>141</v>
+      </c>
       <c r="C70" t="n">
         <v>2014</v>
       </c>
@@ -1674,9 +2148,11 @@
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>73</v>
-      </c>
-      <c r="B71"/>
+        <v>142</v>
+      </c>
+      <c r="B71" t="s">
+        <v>143</v>
+      </c>
       <c r="C71" t="n">
         <v>2014</v>
       </c>
@@ -1686,9 +2162,11 @@
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>74</v>
-      </c>
-      <c r="B72"/>
+        <v>144</v>
+      </c>
+      <c r="B72" t="s">
+        <v>145</v>
+      </c>
       <c r="C72" t="n">
         <v>2014</v>
       </c>
@@ -1698,9 +2176,11 @@
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>75</v>
-      </c>
-      <c r="B73"/>
+        <v>146</v>
+      </c>
+      <c r="B73" t="s">
+        <v>147</v>
+      </c>
       <c r="C73" t="n">
         <v>2014</v>
       </c>
@@ -1710,9 +2190,11 @@
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>76</v>
-      </c>
-      <c r="B74"/>
+        <v>148</v>
+      </c>
+      <c r="B74" t="s">
+        <v>149</v>
+      </c>
       <c r="C74" t="n">
         <v>2014</v>
       </c>
@@ -1722,9 +2204,11 @@
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>77</v>
-      </c>
-      <c r="B75"/>
+        <v>150</v>
+      </c>
+      <c r="B75" t="s">
+        <v>151</v>
+      </c>
       <c r="C75" t="n">
         <v>2014</v>
       </c>
@@ -1734,9 +2218,11 @@
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>78</v>
-      </c>
-      <c r="B76"/>
+        <v>152</v>
+      </c>
+      <c r="B76" t="s">
+        <v>153</v>
+      </c>
       <c r="C76" t="n">
         <v>2014</v>
       </c>
@@ -1746,9 +2232,11 @@
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>79</v>
-      </c>
-      <c r="B77"/>
+        <v>154</v>
+      </c>
+      <c r="B77" t="s">
+        <v>155</v>
+      </c>
       <c r="C77" t="n">
         <v>2014</v>
       </c>
@@ -1758,9 +2246,11 @@
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>80</v>
-      </c>
-      <c r="B78"/>
+        <v>156</v>
+      </c>
+      <c r="B78" t="s">
+        <v>157</v>
+      </c>
       <c r="C78" t="n">
         <v>2014</v>
       </c>
@@ -1770,9 +2260,11 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>81</v>
-      </c>
-      <c r="B79"/>
+        <v>158</v>
+      </c>
+      <c r="B79" t="s">
+        <v>159</v>
+      </c>
       <c r="C79" t="n">
         <v>2014</v>
       </c>
@@ -1782,9 +2274,11 @@
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>82</v>
-      </c>
-      <c r="B80"/>
+        <v>160</v>
+      </c>
+      <c r="B80" t="s">
+        <v>161</v>
+      </c>
       <c r="C80" t="n">
         <v>2014</v>
       </c>
@@ -1794,9 +2288,11 @@
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>83</v>
-      </c>
-      <c r="B81"/>
+        <v>162</v>
+      </c>
+      <c r="B81" t="s">
+        <v>163</v>
+      </c>
       <c r="C81" t="n">
         <v>2014</v>
       </c>
@@ -1806,9 +2302,11 @@
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>84</v>
-      </c>
-      <c r="B82"/>
+        <v>164</v>
+      </c>
+      <c r="B82" t="s">
+        <v>165</v>
+      </c>
       <c r="C82" t="n">
         <v>2014</v>
       </c>
@@ -1818,9 +2316,11 @@
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>85</v>
-      </c>
-      <c r="B83"/>
+        <v>166</v>
+      </c>
+      <c r="B83" t="s">
+        <v>167</v>
+      </c>
       <c r="C83" t="n">
         <v>2014</v>
       </c>
@@ -1830,9 +2330,11 @@
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>86</v>
-      </c>
-      <c r="B84"/>
+        <v>168</v>
+      </c>
+      <c r="B84" t="s">
+        <v>169</v>
+      </c>
       <c r="C84" t="n">
         <v>2014</v>
       </c>
@@ -1842,9 +2344,11 @@
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>87</v>
-      </c>
-      <c r="B85"/>
+        <v>170</v>
+      </c>
+      <c r="B85" t="s">
+        <v>171</v>
+      </c>
       <c r="C85" t="n">
         <v>2014</v>
       </c>
@@ -1854,9 +2358,11 @@
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>88</v>
-      </c>
-      <c r="B86"/>
+        <v>172</v>
+      </c>
+      <c r="B86" t="s">
+        <v>173</v>
+      </c>
       <c r="C86" t="n">
         <v>2014</v>
       </c>
@@ -1866,9 +2372,11 @@
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>89</v>
-      </c>
-      <c r="B87"/>
+        <v>174</v>
+      </c>
+      <c r="B87" t="s">
+        <v>175</v>
+      </c>
       <c r="C87" t="n">
         <v>2014</v>
       </c>
@@ -1878,9 +2386,11 @@
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>90</v>
-      </c>
-      <c r="B88"/>
+        <v>176</v>
+      </c>
+      <c r="B88" t="s">
+        <v>177</v>
+      </c>
       <c r="C88" t="n">
         <v>2014</v>
       </c>
@@ -1890,9 +2400,11 @@
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>91</v>
-      </c>
-      <c r="B89"/>
+        <v>178</v>
+      </c>
+      <c r="B89" t="s">
+        <v>179</v>
+      </c>
       <c r="C89" t="n">
         <v>2014</v>
       </c>
@@ -1902,9 +2414,11 @@
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>92</v>
-      </c>
-      <c r="B90"/>
+        <v>180</v>
+      </c>
+      <c r="B90" t="s">
+        <v>181</v>
+      </c>
       <c r="C90" t="n">
         <v>2014</v>
       </c>
@@ -1914,9 +2428,11 @@
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>93</v>
-      </c>
-      <c r="B91"/>
+        <v>182</v>
+      </c>
+      <c r="B91" t="s">
+        <v>183</v>
+      </c>
       <c r="C91" t="n">
         <v>2014</v>
       </c>
@@ -1926,9 +2442,11 @@
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>94</v>
-      </c>
-      <c r="B92"/>
+        <v>184</v>
+      </c>
+      <c r="B92" t="s">
+        <v>185</v>
+      </c>
       <c r="C92" t="n">
         <v>2014</v>
       </c>
@@ -1938,9 +2456,11 @@
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>95</v>
-      </c>
-      <c r="B93"/>
+        <v>186</v>
+      </c>
+      <c r="B93" t="s">
+        <v>187</v>
+      </c>
       <c r="C93" t="n">
         <v>2014</v>
       </c>
@@ -1950,9 +2470,11 @@
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>96</v>
-      </c>
-      <c r="B94"/>
+        <v>188</v>
+      </c>
+      <c r="B94" t="s">
+        <v>189</v>
+      </c>
       <c r="C94" t="n">
         <v>2014</v>
       </c>
@@ -1962,9 +2484,11 @@
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>97</v>
-      </c>
-      <c r="B95"/>
+        <v>190</v>
+      </c>
+      <c r="B95" t="s">
+        <v>191</v>
+      </c>
       <c r="C95" t="n">
         <v>2014</v>
       </c>
@@ -1974,9 +2498,11 @@
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>98</v>
-      </c>
-      <c r="B96"/>
+        <v>192</v>
+      </c>
+      <c r="B96" t="s">
+        <v>193</v>
+      </c>
       <c r="C96" t="n">
         <v>2014</v>
       </c>
@@ -1986,9 +2512,11 @@
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>99</v>
-      </c>
-      <c r="B97"/>
+        <v>194</v>
+      </c>
+      <c r="B97" t="s">
+        <v>195</v>
+      </c>
       <c r="C97" t="n">
         <v>2014</v>
       </c>
@@ -1998,9 +2526,11 @@
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>100</v>
-      </c>
-      <c r="B98"/>
+        <v>196</v>
+      </c>
+      <c r="B98" t="s">
+        <v>197</v>
+      </c>
       <c r="C98" t="n">
         <v>2014</v>
       </c>
@@ -2010,9 +2540,11 @@
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>101</v>
-      </c>
-      <c r="B99"/>
+        <v>198</v>
+      </c>
+      <c r="B99" t="s">
+        <v>199</v>
+      </c>
       <c r="C99" t="n">
         <v>2014</v>
       </c>
@@ -2022,9 +2554,11 @@
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>102</v>
-      </c>
-      <c r="B100"/>
+        <v>200</v>
+      </c>
+      <c r="B100" t="s">
+        <v>201</v>
+      </c>
       <c r="C100" t="n">
         <v>2014</v>
       </c>
@@ -2034,9 +2568,11 @@
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>103</v>
-      </c>
-      <c r="B101"/>
+        <v>202</v>
+      </c>
+      <c r="B101" t="s">
+        <v>203</v>
+      </c>
       <c r="C101" t="n">
         <v>2014</v>
       </c>
@@ -2046,9 +2582,11 @@
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>104</v>
-      </c>
-      <c r="B102"/>
+        <v>204</v>
+      </c>
+      <c r="B102" t="s">
+        <v>205</v>
+      </c>
       <c r="C102" t="n">
         <v>2014</v>
       </c>
@@ -2058,9 +2596,11 @@
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>105</v>
-      </c>
-      <c r="B103"/>
+        <v>206</v>
+      </c>
+      <c r="B103" t="s">
+        <v>207</v>
+      </c>
       <c r="C103" t="n">
         <v>2014</v>
       </c>
@@ -2070,9 +2610,11 @@
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>106</v>
-      </c>
-      <c r="B104"/>
+        <v>208</v>
+      </c>
+      <c r="B104" t="s">
+        <v>209</v>
+      </c>
       <c r="C104" t="n">
         <v>2014</v>
       </c>
@@ -2082,9 +2624,11 @@
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>107</v>
-      </c>
-      <c r="B105"/>
+        <v>210</v>
+      </c>
+      <c r="B105" t="s">
+        <v>211</v>
+      </c>
       <c r="C105" t="n">
         <v>2014</v>
       </c>
@@ -2094,9 +2638,11 @@
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>108</v>
-      </c>
-      <c r="B106"/>
+        <v>212</v>
+      </c>
+      <c r="B106" t="s">
+        <v>213</v>
+      </c>
       <c r="C106" t="n">
         <v>2014</v>
       </c>
@@ -2106,9 +2652,11 @@
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>109</v>
-      </c>
-      <c r="B107"/>
+        <v>214</v>
+      </c>
+      <c r="B107" t="s">
+        <v>215</v>
+      </c>
       <c r="C107" t="n">
         <v>2014</v>
       </c>
@@ -2118,9 +2666,11 @@
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>110</v>
-      </c>
-      <c r="B108"/>
+        <v>216</v>
+      </c>
+      <c r="B108" t="s">
+        <v>217</v>
+      </c>
       <c r="C108" t="n">
         <v>2014</v>
       </c>
@@ -2130,9 +2680,11 @@
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>111</v>
-      </c>
-      <c r="B109"/>
+        <v>218</v>
+      </c>
+      <c r="B109" t="s">
+        <v>219</v>
+      </c>
       <c r="C109" t="n">
         <v>2014</v>
       </c>
@@ -2142,9 +2694,11 @@
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>112</v>
-      </c>
-      <c r="B110"/>
+        <v>220</v>
+      </c>
+      <c r="B110" t="s">
+        <v>221</v>
+      </c>
       <c r="C110" t="n">
         <v>2014</v>
       </c>
@@ -2154,9 +2708,11 @@
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>113</v>
-      </c>
-      <c r="B111"/>
+        <v>222</v>
+      </c>
+      <c r="B111" t="s">
+        <v>223</v>
+      </c>
       <c r="C111" t="n">
         <v>2014</v>
       </c>
@@ -2166,9 +2722,11 @@
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>114</v>
-      </c>
-      <c r="B112"/>
+        <v>224</v>
+      </c>
+      <c r="B112" t="s">
+        <v>225</v>
+      </c>
       <c r="C112" t="n">
         <v>2014</v>
       </c>
@@ -2178,9 +2736,11 @@
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>115</v>
-      </c>
-      <c r="B113"/>
+        <v>226</v>
+      </c>
+      <c r="B113" t="s">
+        <v>227</v>
+      </c>
       <c r="C113" t="n">
         <v>2014</v>
       </c>
@@ -2207,7 +2767,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>116</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2">
@@ -2220,7 +2780,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="n">
         <v>3.5</v>
@@ -2228,7 +2788,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" t="n">
         <v>4.2</v>
@@ -2236,7 +2796,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" t="n">
         <v>4.2</v>
@@ -2244,7 +2804,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B6" t="n">
         <v>3.8</v>
@@ -2252,7 +2812,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B7" t="n">
         <v>4.1</v>
@@ -2260,7 +2820,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B8" t="n">
         <v>4.4</v>
@@ -2268,7 +2828,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B9" t="n">
         <v>4</v>
@@ -2276,7 +2836,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B10" t="n">
         <v>4.8</v>
@@ -2284,7 +2844,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B11" t="n">
         <v>4.4</v>
@@ -2292,7 +2852,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B12" t="n">
         <v>4.5</v>
@@ -2300,7 +2860,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B13" t="n">
         <v>4.7</v>
@@ -2308,7 +2868,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B14" t="n">
         <v>3.9</v>
@@ -2316,7 +2876,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B15" t="n">
         <v>4.5</v>
@@ -2324,7 +2884,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="B16" t="n">
         <v>4</v>
@@ -2332,7 +2892,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="B17" t="n">
         <v>4.2</v>
@@ -2340,7 +2900,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="B18" t="n">
         <v>4.2</v>
@@ -2348,7 +2908,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="B19" t="n">
         <v>4.3</v>
@@ -2356,7 +2916,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="B20" t="n">
         <v>4.6</v>
@@ -2364,7 +2924,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="B21" t="n">
         <v>3.4</v>
@@ -2372,7 +2932,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="B22" t="n">
         <v>4.5</v>
@@ -2380,7 +2940,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="B23" t="n">
         <v>4.3</v>
@@ -2388,7 +2948,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="B24" t="n">
         <v>4.4</v>
@@ -2396,7 +2956,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="B25" t="n">
         <v>4.4</v>
@@ -2404,7 +2964,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="B26" t="n">
         <v>5.1</v>
@@ -2412,7 +2972,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="B27" t="n">
         <v>4.9</v>
@@ -2420,7 +2980,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="B28" t="n">
         <v>4.9</v>
@@ -2428,7 +2988,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="B29" t="n">
         <v>4.4</v>
@@ -2436,7 +2996,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="B30" t="n">
         <v>5.2</v>
@@ -2444,7 +3004,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="B31" t="n">
         <v>4.8</v>
@@ -2452,7 +3012,7 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="B32" t="n">
         <v>5.3</v>
@@ -2460,7 +3020,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="B33" t="n">
         <v>5.8</v>
@@ -2468,7 +3028,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="B34" t="n">
         <v>4.4</v>
@@ -2476,7 +3036,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="B35" t="n">
         <v>5.7</v>
@@ -2484,7 +3044,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="B36" t="n">
         <v>5.3</v>
@@ -2492,7 +3052,7 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="B37" t="n">
         <v>5</v>
@@ -2500,7 +3060,7 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="B38" t="n">
         <v>5.5</v>
@@ -2508,7 +3068,7 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="B39" t="n">
         <v>4.9</v>
@@ -2516,7 +3076,7 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="B40" t="n">
         <v>4.4</v>
@@ -2524,7 +3084,7 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>82</v>
       </c>
       <c r="B41" t="n">
         <v>5.6</v>
@@ -2532,7 +3092,7 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="B42" t="n">
         <v>5.6</v>
@@ -2540,7 +3100,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="B43" t="n">
         <v>5.7</v>
@@ -2548,7 +3108,7 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="B44" t="n">
         <v>5.7</v>
@@ -2556,7 +3116,7 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>90</v>
       </c>
       <c r="B45" t="n">
         <v>5.3</v>
@@ -2564,7 +3124,7 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="B46" t="n">
         <v>5.5</v>
@@ -2572,7 +3132,7 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="B47" t="n">
         <v>5.4</v>
@@ -2580,7 +3140,7 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>50</v>
+        <v>96</v>
       </c>
       <c r="B48" t="n">
         <v>4.8</v>
@@ -2588,7 +3148,7 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>98</v>
       </c>
       <c r="B49" t="n">
         <v>5.7</v>
@@ -2596,7 +3156,7 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="B50" t="n">
         <v>5.2</v>
@@ -2604,7 +3164,7 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="B51" t="n">
         <v>5.3</v>
@@ -2612,7 +3172,7 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>54</v>
+        <v>104</v>
       </c>
       <c r="B52" t="n">
         <v>5.6</v>
@@ -2620,7 +3180,7 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>106</v>
       </c>
       <c r="B53" t="n">
         <v>5.2</v>
@@ -2628,7 +3188,7 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="B54" t="n">
         <v>5.3</v>
@@ -2636,7 +3196,7 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>110</v>
       </c>
       <c r="B55" t="n">
         <v>4.9</v>
@@ -2644,7 +3204,7 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="B56" t="n">
         <v>6</v>
@@ -2652,7 +3212,7 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>114</v>
       </c>
       <c r="B57" t="n">
         <v>5.9</v>
@@ -2660,7 +3220,7 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>60</v>
+        <v>116</v>
       </c>
       <c r="B58" t="n">
         <v>5.5</v>
@@ -2668,7 +3228,7 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>61</v>
+        <v>118</v>
       </c>
       <c r="B59" t="n">
         <v>5.1</v>
@@ -2676,7 +3236,7 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>120</v>
       </c>
       <c r="B60" t="n">
         <v>5.3</v>
@@ -2684,7 +3244,7 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>63</v>
+        <v>122</v>
       </c>
       <c r="B61" t="n">
         <v>5</v>
@@ -2692,7 +3252,7 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>64</v>
+        <v>124</v>
       </c>
       <c r="B62" t="n">
         <v>5.1</v>
@@ -2700,7 +3260,7 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>65</v>
+        <v>126</v>
       </c>
       <c r="B63" t="n">
         <v>6.3</v>
@@ -2708,7 +3268,7 @@
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>66</v>
+        <v>128</v>
       </c>
       <c r="B64" t="n">
         <v>4.5</v>
@@ -2716,7 +3276,7 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>67</v>
+        <v>130</v>
       </c>
       <c r="B65" t="n">
         <v>4.4</v>
@@ -2724,7 +3284,7 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>68</v>
+        <v>132</v>
       </c>
       <c r="B66" t="n">
         <v>5.3</v>
@@ -2732,7 +3292,7 @@
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="B67" t="n">
         <v>5.1</v>
@@ -2740,7 +3300,7 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>70</v>
+        <v>136</v>
       </c>
       <c r="B68" t="n">
         <v>5.7</v>
@@ -2748,7 +3308,7 @@
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>71</v>
+        <v>138</v>
       </c>
       <c r="B69" t="n">
         <v>5.2</v>
@@ -2756,7 +3316,7 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
       <c r="B70" t="n">
         <v>7.5</v>
@@ -2764,7 +3324,7 @@
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>73</v>
+        <v>142</v>
       </c>
       <c r="B71" t="n">
         <v>5.9</v>
@@ -2772,7 +3332,7 @@
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>74</v>
+        <v>144</v>
       </c>
       <c r="B72" t="n">
         <v>5.2</v>
@@ -2780,7 +3340,7 @@
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>75</v>
+        <v>146</v>
       </c>
       <c r="B73" t="n">
         <v>5</v>
@@ -2788,7 +3348,7 @@
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>76</v>
+        <v>148</v>
       </c>
       <c r="B74" t="n">
         <v>5.2</v>
@@ -2796,7 +3356,7 @@
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>77</v>
+        <v>150</v>
       </c>
       <c r="B75" t="n">
         <v>5.6</v>
@@ -2804,7 +3364,7 @@
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>78</v>
+        <v>152</v>
       </c>
       <c r="B76" t="n">
         <v>6.7</v>
@@ -2812,7 +3372,7 @@
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>79</v>
+        <v>154</v>
       </c>
       <c r="B77" t="n">
         <v>5.1</v>
@@ -2820,7 +3380,7 @@
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>80</v>
+        <v>156</v>
       </c>
       <c r="B78" t="n">
         <v>5</v>
@@ -2828,7 +3388,7 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>81</v>
+        <v>158</v>
       </c>
       <c r="B79" t="n">
         <v>5.2</v>
@@ -2836,7 +3396,7 @@
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>82</v>
+        <v>160</v>
       </c>
       <c r="B80" t="n">
         <v>4.9</v>
@@ -2844,7 +3404,7 @@
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>83</v>
+        <v>162</v>
       </c>
       <c r="B81" t="n">
         <v>6.2</v>
@@ -2852,7 +3412,7 @@
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>84</v>
+        <v>164</v>
       </c>
       <c r="B82" t="n">
         <v>4.9</v>
@@ -2860,7 +3420,7 @@
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>85</v>
+        <v>166</v>
       </c>
       <c r="B83" t="n">
         <v>4.9</v>
@@ -2868,7 +3428,7 @@
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>86</v>
+        <v>168</v>
       </c>
       <c r="B84" t="n">
         <v>5.3</v>
@@ -2876,7 +3436,7 @@
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>87</v>
+        <v>170</v>
       </c>
       <c r="B85" t="n">
         <v>5</v>
@@ -2884,7 +3444,7 @@
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>88</v>
+        <v>172</v>
       </c>
       <c r="B86" t="n">
         <v>4.7</v>
@@ -2892,7 +3452,7 @@
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>89</v>
+        <v>174</v>
       </c>
       <c r="B87" t="n">
         <v>4.7</v>
@@ -2900,7 +3460,7 @@
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>90</v>
+        <v>176</v>
       </c>
       <c r="B88" t="n">
         <v>5</v>
@@ -2908,7 +3468,7 @@
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>91</v>
+        <v>178</v>
       </c>
       <c r="B89" t="n">
         <v>4.4</v>
@@ -2916,7 +3476,7 @@
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>92</v>
+        <v>180</v>
       </c>
       <c r="B90" t="n">
         <v>4.5</v>
@@ -2924,7 +3484,7 @@
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>93</v>
+        <v>182</v>
       </c>
       <c r="B91" t="n">
         <v>4.4</v>
@@ -2932,7 +3492,7 @@
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>94</v>
+        <v>184</v>
       </c>
       <c r="B92" t="n">
         <v>4.3</v>
@@ -2940,7 +3500,7 @@
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>95</v>
+        <v>186</v>
       </c>
       <c r="B93" t="n">
         <v>4.9</v>
@@ -2948,7 +3508,7 @@
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>96</v>
+        <v>188</v>
       </c>
       <c r="B94" t="n">
         <v>4.7</v>
@@ -2956,7 +3516,7 @@
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>97</v>
+        <v>190</v>
       </c>
       <c r="B95" t="n">
         <v>4.5</v>
@@ -2964,7 +3524,7 @@
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>98</v>
+        <v>192</v>
       </c>
       <c r="B96" t="n">
         <v>4.4</v>
@@ -2972,7 +3532,7 @@
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>99</v>
+        <v>194</v>
       </c>
       <c r="B97" t="n">
         <v>4.1</v>
@@ -2980,7 +3540,7 @@
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>100</v>
+        <v>196</v>
       </c>
       <c r="B98" t="n">
         <v>4.7</v>
@@ -2988,7 +3548,7 @@
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>101</v>
+        <v>198</v>
       </c>
       <c r="B99" t="n">
         <v>4.5</v>
@@ -2996,7 +3556,7 @@
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>102</v>
+        <v>200</v>
       </c>
       <c r="B100" t="n">
         <v>4.6</v>
@@ -3004,7 +3564,7 @@
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>103</v>
+        <v>202</v>
       </c>
       <c r="B101" t="n">
         <v>4.5</v>
@@ -3012,7 +3572,7 @@
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>104</v>
+        <v>204</v>
       </c>
       <c r="B102" t="n">
         <v>4.6</v>
@@ -3020,7 +3580,7 @@
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>105</v>
+        <v>206</v>
       </c>
       <c r="B103" t="n">
         <v>5</v>
@@ -3028,7 +3588,7 @@
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>106</v>
+        <v>208</v>
       </c>
       <c r="B104" t="n">
         <v>4.5</v>
@@ -3036,7 +3596,7 @@
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>107</v>
+        <v>210</v>
       </c>
       <c r="B105" t="n">
         <v>4.7</v>
@@ -3044,7 +3604,7 @@
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>108</v>
+        <v>212</v>
       </c>
       <c r="B106" t="n">
         <v>4.8</v>
@@ -3052,7 +3612,7 @@
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>109</v>
+        <v>214</v>
       </c>
       <c r="B107" t="n">
         <v>4.8</v>
@@ -3060,7 +3620,7 @@
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>110</v>
+        <v>216</v>
       </c>
       <c r="B108" t="n">
         <v>5</v>
@@ -3068,7 +3628,7 @@
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>111</v>
+        <v>218</v>
       </c>
       <c r="B109" t="n">
         <v>4.7</v>
@@ -3076,7 +3636,7 @@
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>112</v>
+        <v>220</v>
       </c>
       <c r="B110" t="n">
         <v>4.6</v>
@@ -3084,7 +3644,7 @@
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>113</v>
+        <v>222</v>
       </c>
       <c r="B111" t="n">
         <v>4.8</v>
@@ -3092,7 +3652,7 @@
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>114</v>
+        <v>224</v>
       </c>
       <c r="B112" t="n">
         <v>4.4</v>
@@ -3100,7 +3660,7 @@
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>115</v>
+        <v>226</v>
       </c>
       <c r="B113" t="n">
         <v>4.4</v>

</xml_diff>